<commit_message>
Added highlighted class diagrams, updated and exported mapping spreadsheets
</commit_message>
<xml_diff>
--- a/Master NIEM Document/Mapping_Spreadsheets/00 Crash Driver Report Fresh.xlsx
+++ b/Master NIEM Document/Mapping_Spreadsheets/00 Crash Driver Report Fresh.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - CrashDriverReport Com" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Crash Driver Report" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
-    <t>CrashDriverReport Complete</t>
+    <t>Crash Driver Report</t>
   </si>
   <si>
     <t>Class</t>
@@ -1506,7 +1506,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:P24"/>
+  <dimension ref="A2:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
@@ -2069,19 +2069,17 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="12">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s" s="12">
-        <v>52</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B20" s="13"/>
       <c r="C20" t="s" s="14">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D20" t="s" s="12">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s" s="15">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="F20" s="16"/>
       <c r="G20" s="17"/>
@@ -2099,15 +2097,17 @@
       <c r="A21" t="s" s="12">
         <v>54</v>
       </c>
-      <c r="B21" s="13"/>
+      <c r="B21" t="s" s="12">
+        <v>57</v>
+      </c>
       <c r="C21" t="s" s="14">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s" s="12">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s" s="15">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="17"/>
@@ -2126,13 +2126,13 @@
         <v>54</v>
       </c>
       <c r="B22" t="s" s="12">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s" s="14">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s" s="12">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s" s="15">
         <v>19</v>
@@ -2154,10 +2154,10 @@
         <v>54</v>
       </c>
       <c r="B23" t="s" s="12">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s" s="14">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s" s="12">
         <v>49</v>
@@ -2177,34 +2177,6 @@
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
     </row>
-    <row r="24" ht="20.05" customHeight="1">
-      <c r="A24" t="s" s="12">
-        <v>54</v>
-      </c>
-      <c r="B24" t="s" s="12">
-        <v>61</v>
-      </c>
-      <c r="C24" t="s" s="14">
-        <v>62</v>
-      </c>
-      <c r="D24" t="s" s="12">
-        <v>49</v>
-      </c>
-      <c r="E24" t="s" s="15">
-        <v>19</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>

</xml_diff>